<commit_message>
students list prints classrooms now too
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/excelResources/Students.xlsx
+++ b/backend/src/main/resources/excelResources/Students.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Bilkent ID</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Classrooms</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -366,10 +369,11 @@
     <col min="2" max="2" width="24.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="20.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -382,8 +386,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>